<commit_message>
merge file and aspx
</commit_message>
<xml_diff>
--- a/TeplosilaWeb/Content/properties/gtrv.xlsx
+++ b/TeplosilaWeb/Content/properties/gtrv.xlsx
@@ -87,7 +87,7 @@
     <t>TSL-3000-60-1R-230-IP67</t>
   </si>
   <si>
-    <t>TRV, TRV-P, TRV-T</t>
+    <t>TRV</t>
   </si>
 </sst>
 </file>
@@ -206,6 +206,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -215,13 +222,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -506,7 +506,7 @@
   <dimension ref="A1:M31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q21" sqref="Q21"/>
+      <selection activeCell="R19" sqref="R19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -516,21 +516,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-      <c r="H1" s="9"/>
-      <c r="I1" s="9"/>
-      <c r="J1" s="9"/>
-      <c r="K1" s="9"/>
-      <c r="L1" s="9"/>
-      <c r="M1" s="9"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="12"/>
+      <c r="I1" s="12"/>
+      <c r="J1" s="12"/>
+      <c r="K1" s="12"/>
+      <c r="L1" s="12"/>
+      <c r="M1" s="12"/>
     </row>
     <row r="2" spans="1:13" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
@@ -539,19 +539,19 @@
       <c r="B2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7"/>
-      <c r="I2" s="7"/>
-      <c r="J2" s="7"/>
-      <c r="K2" s="7"/>
-      <c r="L2" s="7"/>
-      <c r="M2" s="7"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="10"/>
+      <c r="H2" s="10"/>
+      <c r="I2" s="10"/>
+      <c r="J2" s="10"/>
+      <c r="K2" s="10"/>
+      <c r="L2" s="10"/>
+      <c r="M2" s="10"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="6">
@@ -680,20 +680,20 @@
       <c r="A6" s="6">
         <v>4</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="8"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8"/>
-      <c r="F6" s="8"/>
-      <c r="G6" s="8"/>
-      <c r="H6" s="8"/>
-      <c r="I6" s="8"/>
-      <c r="J6" s="8"/>
-      <c r="K6" s="8"/>
-      <c r="L6" s="8"/>
-      <c r="M6" s="8"/>
+      <c r="C6" s="11"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="11"/>
+      <c r="G6" s="11"/>
+      <c r="H6" s="11"/>
+      <c r="I6" s="11"/>
+      <c r="J6" s="11"/>
+      <c r="K6" s="11"/>
+      <c r="L6" s="11"/>
+      <c r="M6" s="11"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="6">
@@ -703,10 +703,10 @@
         <v>5</v>
       </c>
       <c r="C7" s="2">
-        <v>302</v>
+        <v>305</v>
       </c>
       <c r="D7" s="2">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="E7" s="2">
         <v>313</v>
@@ -734,10 +734,10 @@
         <v>6</v>
       </c>
       <c r="C8" s="2">
-        <v>302</v>
+        <v>305</v>
       </c>
       <c r="D8" s="2">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="E8" s="2">
         <v>313</v>
@@ -942,26 +942,26 @@
         <v>565</v>
       </c>
     </row>
-    <row r="16" spans="1:13" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="10">
+    <row r="16" spans="1:13" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="7">
         <v>14</v>
       </c>
-      <c r="B16" s="11" t="s">
+      <c r="B16" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="C16" s="10"/>
-      <c r="D16" s="10"/>
-      <c r="E16" s="10"/>
-      <c r="F16" s="10"/>
-      <c r="G16" s="10"/>
-      <c r="H16" s="10"/>
-      <c r="I16" s="10"/>
-      <c r="J16" s="10"/>
-      <c r="K16" s="10"/>
-      <c r="L16" s="10">
+      <c r="C16" s="7"/>
+      <c r="D16" s="7"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="7"/>
+      <c r="G16" s="7"/>
+      <c r="H16" s="7"/>
+      <c r="I16" s="7"/>
+      <c r="J16" s="7"/>
+      <c r="K16" s="7"/>
+      <c r="L16" s="7">
         <v>535</v>
       </c>
-      <c r="M16" s="10">
+      <c r="M16" s="7">
         <v>565</v>
       </c>
     </row>
@@ -1015,20 +1015,20 @@
       <c r="A19" s="6">
         <v>17</v>
       </c>
-      <c r="B19" s="8" t="s">
+      <c r="B19" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="C19" s="8"/>
-      <c r="D19" s="8"/>
-      <c r="E19" s="8"/>
-      <c r="F19" s="8"/>
-      <c r="G19" s="8"/>
-      <c r="H19" s="8"/>
-      <c r="I19" s="8"/>
-      <c r="J19" s="8"/>
-      <c r="K19" s="8"/>
-      <c r="L19" s="8"/>
-      <c r="M19" s="8"/>
+      <c r="C19" s="11"/>
+      <c r="D19" s="11"/>
+      <c r="E19" s="11"/>
+      <c r="F19" s="11"/>
+      <c r="G19" s="11"/>
+      <c r="H19" s="11"/>
+      <c r="I19" s="11"/>
+      <c r="J19" s="11"/>
+      <c r="K19" s="11"/>
+      <c r="L19" s="11"/>
+      <c r="M19" s="11"/>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="6">
@@ -1277,26 +1277,26 @@
         <v>72.3</v>
       </c>
     </row>
-    <row r="29" spans="1:13" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="10">
+    <row r="29" spans="1:13" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="7">
         <v>27</v>
       </c>
-      <c r="B29" s="11" t="s">
+      <c r="B29" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="C29" s="10"/>
-      <c r="D29" s="10"/>
-      <c r="E29" s="10"/>
-      <c r="F29" s="10"/>
-      <c r="G29" s="10"/>
-      <c r="H29" s="10"/>
-      <c r="I29" s="10"/>
-      <c r="J29" s="10"/>
-      <c r="K29" s="10"/>
-      <c r="L29" s="10">
+      <c r="C29" s="7"/>
+      <c r="D29" s="7"/>
+      <c r="E29" s="7"/>
+      <c r="F29" s="7"/>
+      <c r="G29" s="7"/>
+      <c r="H29" s="7"/>
+      <c r="I29" s="7"/>
+      <c r="J29" s="7"/>
+      <c r="K29" s="7"/>
+      <c r="L29" s="7">
         <v>54.3</v>
       </c>
-      <c r="M29" s="10">
+      <c r="M29" s="7">
         <v>72.3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added new trv and fixed table and fixed radiobutton
</commit_message>
<xml_diff>
--- a/TeplosilaWeb/Content/properties/gtrv.xlsx
+++ b/TeplosilaWeb/Content/properties/gtrv.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\CSharp\TeploSila_RDT\TeploSila_RDT\TeploSila_2\bin\Debug\properties\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/22451d98f477d1d3/Рабочий стол/RDT/TeplosilaWeb/Content/properties/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="2" documentId="8_{08BDB76B-10D6-4846-95AD-0C69193C8E1B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{E119D0ED-DB60-49D5-8074-864A836D70ED}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
+    <workbookView xWindow="-28920" yWindow="15" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="25">
   <si>
     <t>Наименование параметров,
 единицы измерения</t>
@@ -84,16 +85,28 @@
     <t>TSL-3000-60-1-230-IP67</t>
   </si>
   <si>
+    <t>TRV</t>
+  </si>
+  <si>
+    <t>TSL-1600-25-1T-230-IP67</t>
+  </si>
+  <si>
+    <t>TSL-1600-25-1TR-230-IP67</t>
+  </si>
+  <si>
+    <t>TSL-2200-40-1T-230-IP67</t>
+  </si>
+  <si>
+    <t>TSL-2200-40-1TR-230-IP67</t>
+  </si>
+  <si>
     <t>TSL-3000-60-1R-230-IP67</t>
-  </si>
-  <si>
-    <t>TRV</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -149,7 +162,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -181,12 +194,49 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -198,13 +248,13 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -212,7 +262,15 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -502,103 +560,103 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M31"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:M39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R19" sqref="R19"/>
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="6.7109375" customWidth="1"/>
-    <col min="2" max="2" width="25.28515625" customWidth="1"/>
+    <col min="1" max="1" width="6.6640625" customWidth="1"/>
+    <col min="2" max="2" width="25.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
-      <c r="H1" s="12"/>
-      <c r="I1" s="12"/>
-      <c r="J1" s="12"/>
-      <c r="K1" s="12"/>
-      <c r="L1" s="12"/>
-      <c r="M1" s="12"/>
-    </row>
-    <row r="2" spans="1:13" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A1" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
+      <c r="I1" s="14"/>
+      <c r="J1" s="14"/>
+      <c r="K1" s="14"/>
+      <c r="L1" s="14"/>
+      <c r="M1" s="14"/>
+    </row>
+    <row r="2" spans="1:13" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>17</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="C2" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10"/>
-      <c r="G2" s="10"/>
-      <c r="H2" s="10"/>
-      <c r="I2" s="10"/>
-      <c r="J2" s="10"/>
-      <c r="K2" s="10"/>
-      <c r="L2" s="10"/>
-      <c r="M2" s="10"/>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" s="6">
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
+      <c r="H2" s="12"/>
+      <c r="I2" s="12"/>
+      <c r="J2" s="12"/>
+      <c r="K2" s="12"/>
+      <c r="L2" s="12"/>
+      <c r="M2" s="12"/>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A3" s="5">
         <v>1</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="5">
+      <c r="C3" s="4">
         <v>15</v>
       </c>
-      <c r="D3" s="5">
+      <c r="D3" s="4">
         <v>20</v>
       </c>
-      <c r="E3" s="5">
+      <c r="E3" s="4">
         <v>25</v>
       </c>
-      <c r="F3" s="5">
+      <c r="F3" s="4">
         <v>32</v>
       </c>
-      <c r="G3" s="5">
+      <c r="G3" s="4">
         <v>40</v>
       </c>
-      <c r="H3" s="5">
+      <c r="H3" s="4">
         <v>50</v>
       </c>
-      <c r="I3" s="5">
+      <c r="I3" s="4">
         <v>65</v>
       </c>
-      <c r="J3" s="5">
+      <c r="J3" s="4">
         <v>80</v>
       </c>
-      <c r="K3" s="5">
+      <c r="K3" s="4">
         <v>100</v>
       </c>
-      <c r="L3" s="5">
+      <c r="L3" s="4">
         <v>125</v>
       </c>
-      <c r="M3" s="5">
+      <c r="M3" s="4">
         <v>150</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" s="6">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A4" s="5">
         <v>2</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="6" t="s">
         <v>3</v>
       </c>
       <c r="C4" s="2">
@@ -635,11 +693,11 @@
         <v>480</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" s="6">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A5" s="5">
         <v>3</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="6" t="s">
         <v>4</v>
       </c>
       <c r="C5" s="2">
@@ -676,27 +734,27 @@
         <v>142.5</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="6">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A6" s="5">
         <v>4</v>
       </c>
-      <c r="B6" s="11" t="s">
+      <c r="B6" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="11"/>
-      <c r="D6" s="11"/>
-      <c r="E6" s="11"/>
-      <c r="F6" s="11"/>
-      <c r="G6" s="11"/>
-      <c r="H6" s="11"/>
-      <c r="I6" s="11"/>
-      <c r="J6" s="11"/>
-      <c r="K6" s="11"/>
-      <c r="L6" s="11"/>
-      <c r="M6" s="11"/>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" s="6">
+      <c r="C6" s="13"/>
+      <c r="D6" s="13"/>
+      <c r="E6" s="13"/>
+      <c r="F6" s="13"/>
+      <c r="G6" s="13"/>
+      <c r="H6" s="13"/>
+      <c r="I6" s="13"/>
+      <c r="J6" s="13"/>
+      <c r="K6" s="13"/>
+      <c r="L6" s="13"/>
+      <c r="M6" s="13"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A7" s="5">
         <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
@@ -726,8 +784,8 @@
       <c r="L7" s="2"/>
       <c r="M7" s="2"/>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" s="6">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A8" s="5">
         <v>6</v>
       </c>
       <c r="B8" s="1" t="s">
@@ -757,8 +815,8 @@
       <c r="L8" s="2"/>
       <c r="M8" s="2"/>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" s="6">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A9" s="5">
         <v>7</v>
       </c>
       <c r="B9" s="1" t="s">
@@ -788,8 +846,8 @@
       <c r="L9" s="2"/>
       <c r="M9" s="2"/>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" s="6">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A10" s="5">
         <v>8</v>
       </c>
       <c r="B10" s="1" t="s">
@@ -819,8 +877,8 @@
       <c r="L10" s="2"/>
       <c r="M10" s="2"/>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" s="6">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A11" s="5">
         <v>9</v>
       </c>
       <c r="B11" s="1" t="s">
@@ -844,8 +902,8 @@
       <c r="L11" s="2"/>
       <c r="M11" s="2"/>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" s="6">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A12" s="5">
         <v>10</v>
       </c>
       <c r="B12" s="1" t="s">
@@ -869,8 +927,8 @@
       <c r="L12" s="2"/>
       <c r="M12" s="2"/>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A13" s="6">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A13" s="5">
         <v>11</v>
       </c>
       <c r="B13" s="1" t="s">
@@ -894,8 +952,8 @@
       <c r="L13" s="2"/>
       <c r="M13" s="2"/>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A14" s="6">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A14" s="5">
         <v>12</v>
       </c>
       <c r="B14" s="1" t="s">
@@ -919,8 +977,8 @@
       <c r="L14" s="2"/>
       <c r="M14" s="2"/>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A15" s="6">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A15" s="5">
         <v>13</v>
       </c>
       <c r="B15" s="1" t="s">
@@ -942,12 +1000,12 @@
         <v>565</v>
       </c>
     </row>
-    <row r="16" spans="1:13" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16" s="7">
         <v>14</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="C16" s="7"/>
       <c r="D16" s="7"/>
@@ -965,8 +1023,8 @@
         <v>565</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A17" s="6">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A17" s="5">
         <v>15</v>
       </c>
       <c r="B17" s="1" t="s">
@@ -988,8 +1046,8 @@
         <v>525</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A18" s="6">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A18" s="5">
         <v>16</v>
       </c>
       <c r="B18" s="1" t="s">
@@ -1011,49 +1069,61 @@
         <v>525</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A19" s="6">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A19" s="5">
         <v>17</v>
       </c>
-      <c r="B19" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="C19" s="11"/>
-      <c r="D19" s="11"/>
-      <c r="E19" s="11"/>
-      <c r="F19" s="11"/>
-      <c r="G19" s="11"/>
-      <c r="H19" s="11"/>
-      <c r="I19" s="11"/>
-      <c r="J19" s="11"/>
-      <c r="K19" s="11"/>
-      <c r="L19" s="11"/>
-      <c r="M19" s="11"/>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A20" s="6">
+      <c r="B19" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C19" s="2">
+        <v>305</v>
+      </c>
+      <c r="D19" s="2">
+        <v>305</v>
+      </c>
+      <c r="E19" s="2">
+        <v>313</v>
+      </c>
+      <c r="F19" s="2">
+        <v>323</v>
+      </c>
+      <c r="G19" s="2">
+        <v>332</v>
+      </c>
+      <c r="H19" s="2">
+        <v>337</v>
+      </c>
+      <c r="I19" s="2"/>
+      <c r="J19" s="2"/>
+      <c r="K19" s="2"/>
+      <c r="L19" s="2"/>
+      <c r="M19" s="2"/>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A20" s="5">
         <v>18</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="C20" s="2">
-        <v>6.2</v>
+        <v>305</v>
       </c>
       <c r="D20" s="2">
-        <v>7.7</v>
+        <v>305</v>
       </c>
       <c r="E20" s="2">
-        <v>8.1999999999999993</v>
+        <v>313</v>
       </c>
       <c r="F20" s="2">
-        <v>11.2</v>
+        <v>323</v>
       </c>
       <c r="G20" s="2">
-        <v>13.2</v>
+        <v>332</v>
       </c>
       <c r="H20" s="2">
-        <v>15.2</v>
+        <v>337</v>
       </c>
       <c r="I20" s="2"/>
       <c r="J20" s="2"/>
@@ -1061,205 +1131,205 @@
       <c r="L20" s="2"/>
       <c r="M20" s="2"/>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A21" s="6">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A21" s="5">
         <v>19</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C21" s="2">
-        <v>6.2</v>
-      </c>
-      <c r="D21" s="2">
-        <v>7.7</v>
-      </c>
-      <c r="E21" s="2">
-        <v>8.1999999999999993</v>
-      </c>
-      <c r="F21" s="2">
-        <v>11.2</v>
-      </c>
-      <c r="G21" s="2">
-        <v>13.2</v>
-      </c>
-      <c r="H21" s="2">
-        <v>15.2</v>
-      </c>
-      <c r="I21" s="2"/>
-      <c r="J21" s="2"/>
-      <c r="K21" s="2"/>
+        <v>22</v>
+      </c>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+      <c r="G21" s="2"/>
+      <c r="H21" s="2"/>
+      <c r="I21" s="2">
+        <v>395</v>
+      </c>
+      <c r="J21" s="2">
+        <v>408</v>
+      </c>
+      <c r="K21" s="2">
+        <v>445</v>
+      </c>
       <c r="L21" s="2"/>
       <c r="M21" s="2"/>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A22" s="6">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A22" s="5">
         <v>20</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C22" s="2">
-        <v>6.7</v>
-      </c>
-      <c r="D22" s="2">
-        <v>8.1999999999999993</v>
-      </c>
-      <c r="E22" s="2">
-        <v>8.6999999999999993</v>
-      </c>
-      <c r="F22" s="2">
-        <v>11.7</v>
-      </c>
-      <c r="G22" s="2">
-        <v>13.7</v>
-      </c>
-      <c r="H22" s="2">
-        <v>15.7</v>
-      </c>
-      <c r="I22" s="2"/>
-      <c r="J22" s="2"/>
-      <c r="K22" s="2"/>
+        <v>23</v>
+      </c>
+      <c r="C22" s="2"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+      <c r="G22" s="2"/>
+      <c r="H22" s="2"/>
+      <c r="I22" s="2">
+        <v>395</v>
+      </c>
+      <c r="J22" s="2">
+        <v>408</v>
+      </c>
+      <c r="K22" s="2">
+        <v>445</v>
+      </c>
       <c r="L22" s="2"/>
       <c r="M22" s="2"/>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A23" s="6">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A23" s="5">
         <v>21</v>
       </c>
-      <c r="B23" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C23" s="2">
-        <v>6.7</v>
-      </c>
-      <c r="D23" s="2">
+      <c r="B23" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C23" s="10"/>
+      <c r="D23" s="10"/>
+      <c r="E23" s="10"/>
+      <c r="F23" s="10"/>
+      <c r="G23" s="10"/>
+      <c r="H23" s="10"/>
+      <c r="I23" s="10"/>
+      <c r="J23" s="10"/>
+      <c r="K23" s="10"/>
+      <c r="L23" s="10"/>
+      <c r="M23" s="11"/>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A24" s="5">
+        <v>22</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C24" s="2">
+        <v>6.2</v>
+      </c>
+      <c r="D24" s="2">
+        <v>7.7</v>
+      </c>
+      <c r="E24" s="2">
         <v>8.1999999999999993</v>
       </c>
-      <c r="E23" s="2">
-        <v>8.6999999999999993</v>
-      </c>
-      <c r="F23" s="2">
-        <v>11.7</v>
-      </c>
-      <c r="G23" s="2">
-        <v>13.7</v>
-      </c>
-      <c r="H23" s="2">
-        <v>15.7</v>
-      </c>
-      <c r="I23" s="2"/>
-      <c r="J23" s="2"/>
-      <c r="K23" s="2"/>
-      <c r="L23" s="2"/>
-      <c r="M23" s="2"/>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A24" s="6">
-        <v>22</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C24" s="2"/>
-      <c r="D24" s="2"/>
-      <c r="E24" s="2"/>
-      <c r="F24" s="2"/>
-      <c r="G24" s="2"/>
-      <c r="H24" s="2"/>
-      <c r="I24" s="2">
-        <v>24.5</v>
-      </c>
-      <c r="J24" s="2">
-        <v>32.5</v>
-      </c>
-      <c r="K24" s="2">
-        <v>39.5</v>
-      </c>
+      <c r="F24" s="2">
+        <v>11.2</v>
+      </c>
+      <c r="G24" s="2">
+        <v>13.2</v>
+      </c>
+      <c r="H24" s="2">
+        <v>15.2</v>
+      </c>
+      <c r="I24" s="2"/>
+      <c r="J24" s="2"/>
+      <c r="K24" s="2"/>
       <c r="L24" s="2"/>
       <c r="M24" s="2"/>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A25" s="6">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A25" s="5">
         <v>23</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C25" s="2"/>
-      <c r="D25" s="2"/>
-      <c r="E25" s="2"/>
-      <c r="F25" s="2"/>
-      <c r="G25" s="2"/>
-      <c r="H25" s="2"/>
-      <c r="I25" s="2">
-        <v>24.5</v>
-      </c>
-      <c r="J25" s="2">
-        <v>32.5</v>
-      </c>
-      <c r="K25" s="2">
-        <v>39.5</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="C25" s="2">
+        <v>6.2</v>
+      </c>
+      <c r="D25" s="2">
+        <v>7.7</v>
+      </c>
+      <c r="E25" s="2">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="F25" s="2">
+        <v>11.2</v>
+      </c>
+      <c r="G25" s="2">
+        <v>13.2</v>
+      </c>
+      <c r="H25" s="2">
+        <v>15.2</v>
+      </c>
+      <c r="I25" s="2"/>
+      <c r="J25" s="2"/>
+      <c r="K25" s="2"/>
       <c r="L25" s="2"/>
       <c r="M25" s="2"/>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A26" s="6">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A26" s="5">
         <v>24</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C26" s="2"/>
-      <c r="D26" s="2"/>
-      <c r="E26" s="2"/>
-      <c r="F26" s="2"/>
-      <c r="G26" s="2"/>
-      <c r="H26" s="2"/>
-      <c r="I26" s="2">
-        <v>24.5</v>
-      </c>
-      <c r="J26" s="2">
-        <v>32.5</v>
-      </c>
-      <c r="K26" s="2">
-        <v>39.5</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="C26" s="2">
+        <v>6.7</v>
+      </c>
+      <c r="D26" s="2">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="E26" s="2">
+        <v>8.6999999999999993</v>
+      </c>
+      <c r="F26" s="2">
+        <v>11.7</v>
+      </c>
+      <c r="G26" s="2">
+        <v>13.7</v>
+      </c>
+      <c r="H26" s="2">
+        <v>15.7</v>
+      </c>
+      <c r="I26" s="2"/>
+      <c r="J26" s="2"/>
+      <c r="K26" s="2"/>
       <c r="L26" s="2"/>
       <c r="M26" s="2"/>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A27" s="6">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A27" s="5">
         <v>25</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C27" s="2"/>
-      <c r="D27" s="2"/>
-      <c r="E27" s="2"/>
-      <c r="F27" s="2"/>
-      <c r="G27" s="2"/>
-      <c r="H27" s="2"/>
-      <c r="I27" s="2">
-        <v>24.5</v>
-      </c>
-      <c r="J27" s="2">
-        <v>32.5</v>
-      </c>
-      <c r="K27" s="2">
-        <v>39.5</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="C27" s="2">
+        <v>6.7</v>
+      </c>
+      <c r="D27" s="2">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="E27" s="2">
+        <v>8.6999999999999993</v>
+      </c>
+      <c r="F27" s="2">
+        <v>11.7</v>
+      </c>
+      <c r="G27" s="2">
+        <v>13.7</v>
+      </c>
+      <c r="H27" s="2">
+        <v>15.7</v>
+      </c>
+      <c r="I27" s="2"/>
+      <c r="J27" s="2"/>
+      <c r="K27" s="2"/>
       <c r="L27" s="2"/>
       <c r="M27" s="2"/>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A28" s="6">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A28" s="5">
         <v>26</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
@@ -1267,45 +1337,49 @@
       <c r="F28" s="2"/>
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
-      <c r="I28" s="2"/>
-      <c r="J28" s="2"/>
-      <c r="K28" s="2"/>
-      <c r="L28" s="2">
-        <v>54.3</v>
-      </c>
-      <c r="M28" s="2">
-        <v>72.3</v>
-      </c>
-    </row>
-    <row r="29" spans="1:13" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="7">
+      <c r="I28" s="2">
+        <v>24.5</v>
+      </c>
+      <c r="J28" s="2">
+        <v>32.5</v>
+      </c>
+      <c r="K28" s="2">
+        <v>39.5</v>
+      </c>
+      <c r="L28" s="2"/>
+      <c r="M28" s="2"/>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A29" s="5">
         <v>27</v>
       </c>
-      <c r="B29" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="C29" s="7"/>
-      <c r="D29" s="7"/>
-      <c r="E29" s="7"/>
-      <c r="F29" s="7"/>
-      <c r="G29" s="7"/>
-      <c r="H29" s="7"/>
-      <c r="I29" s="7"/>
-      <c r="J29" s="7"/>
-      <c r="K29" s="7"/>
-      <c r="L29" s="7">
-        <v>54.3</v>
-      </c>
-      <c r="M29" s="7">
-        <v>72.3</v>
-      </c>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A30" s="6">
+      <c r="B29" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C29" s="2"/>
+      <c r="D29" s="2"/>
+      <c r="E29" s="2"/>
+      <c r="F29" s="2"/>
+      <c r="G29" s="2"/>
+      <c r="H29" s="2"/>
+      <c r="I29" s="2">
+        <v>24.5</v>
+      </c>
+      <c r="J29" s="2">
+        <v>32.5</v>
+      </c>
+      <c r="K29" s="2">
+        <v>39.5</v>
+      </c>
+      <c r="L29" s="2"/>
+      <c r="M29" s="2"/>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A30" s="5">
         <v>28</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C30" s="2"/>
       <c r="D30" s="2"/>
@@ -1313,22 +1387,24 @@
       <c r="F30" s="2"/>
       <c r="G30" s="2"/>
       <c r="H30" s="2"/>
-      <c r="I30" s="2"/>
-      <c r="J30" s="2"/>
-      <c r="K30" s="2"/>
-      <c r="L30" s="2">
-        <v>53</v>
-      </c>
-      <c r="M30" s="2">
-        <v>71.3</v>
-      </c>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A31" s="6">
+      <c r="I30" s="2">
+        <v>24.5</v>
+      </c>
+      <c r="J30" s="2">
+        <v>32.5</v>
+      </c>
+      <c r="K30" s="2">
+        <v>39.5</v>
+      </c>
+      <c r="L30" s="2"/>
+      <c r="M30" s="2"/>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A31" s="5">
         <v>29</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C31" s="2"/>
       <c r="D31" s="2"/>
@@ -1336,21 +1412,226 @@
       <c r="F31" s="2"/>
       <c r="G31" s="2"/>
       <c r="H31" s="2"/>
-      <c r="I31" s="2"/>
-      <c r="J31" s="2"/>
-      <c r="K31" s="2"/>
-      <c r="L31" s="2">
+      <c r="I31" s="2">
+        <v>24.5</v>
+      </c>
+      <c r="J31" s="2">
+        <v>32.5</v>
+      </c>
+      <c r="K31" s="2">
+        <v>39.5</v>
+      </c>
+      <c r="L31" s="2"/>
+      <c r="M31" s="2"/>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A32" s="5">
+        <v>30</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C32" s="2"/>
+      <c r="D32" s="2"/>
+      <c r="E32" s="2"/>
+      <c r="F32" s="2"/>
+      <c r="G32" s="2"/>
+      <c r="H32" s="2"/>
+      <c r="I32" s="2"/>
+      <c r="J32" s="2"/>
+      <c r="K32" s="2"/>
+      <c r="L32" s="2">
+        <v>54.3</v>
+      </c>
+      <c r="M32" s="2">
+        <v>72.3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A33" s="7">
+        <v>27</v>
+      </c>
+      <c r="B33" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C33" s="7"/>
+      <c r="D33" s="7"/>
+      <c r="E33" s="7"/>
+      <c r="F33" s="7"/>
+      <c r="G33" s="7"/>
+      <c r="H33" s="7"/>
+      <c r="I33" s="7"/>
+      <c r="J33" s="7"/>
+      <c r="K33" s="7"/>
+      <c r="L33" s="7">
+        <v>54.3</v>
+      </c>
+      <c r="M33" s="7">
+        <v>72.3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A34" s="5">
+        <v>32</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C34" s="2"/>
+      <c r="D34" s="2"/>
+      <c r="E34" s="2"/>
+      <c r="F34" s="2"/>
+      <c r="G34" s="2"/>
+      <c r="H34" s="2"/>
+      <c r="I34" s="2"/>
+      <c r="J34" s="2"/>
+      <c r="K34" s="2"/>
+      <c r="L34" s="2">
         <v>53</v>
       </c>
-      <c r="M31" s="2">
+      <c r="M34" s="2">
         <v>71.3</v>
       </c>
     </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A35" s="5">
+        <v>33</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C35" s="2"/>
+      <c r="D35" s="2"/>
+      <c r="E35" s="2"/>
+      <c r="F35" s="2"/>
+      <c r="G35" s="2"/>
+      <c r="H35" s="2"/>
+      <c r="I35" s="2"/>
+      <c r="J35" s="2"/>
+      <c r="K35" s="2"/>
+      <c r="L35" s="2">
+        <v>53</v>
+      </c>
+      <c r="M35" s="2">
+        <v>71.3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A36" s="5">
+        <v>34</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C36" s="2">
+        <v>6.2</v>
+      </c>
+      <c r="D36" s="2">
+        <v>7.7</v>
+      </c>
+      <c r="E36" s="2">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="F36" s="2">
+        <v>11.2</v>
+      </c>
+      <c r="G36" s="2">
+        <v>13.2</v>
+      </c>
+      <c r="H36" s="2">
+        <v>15.2</v>
+      </c>
+      <c r="I36" s="2"/>
+      <c r="J36" s="2"/>
+      <c r="K36" s="2"/>
+      <c r="L36" s="2"/>
+      <c r="M36" s="2"/>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A37" s="5">
+        <v>35</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C37" s="2">
+        <v>6.2</v>
+      </c>
+      <c r="D37" s="2">
+        <v>7.7</v>
+      </c>
+      <c r="E37" s="2">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="F37" s="2">
+        <v>11.2</v>
+      </c>
+      <c r="G37" s="2">
+        <v>13.2</v>
+      </c>
+      <c r="H37" s="2">
+        <v>15.2</v>
+      </c>
+      <c r="I37" s="2"/>
+      <c r="J37" s="2"/>
+      <c r="K37" s="2"/>
+      <c r="L37" s="2"/>
+      <c r="M37" s="2"/>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A38" s="5">
+        <v>36</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C38" s="2"/>
+      <c r="D38" s="2"/>
+      <c r="E38" s="2"/>
+      <c r="F38" s="2"/>
+      <c r="G38" s="2"/>
+      <c r="H38" s="2"/>
+      <c r="I38" s="2">
+        <v>24.5</v>
+      </c>
+      <c r="J38" s="2">
+        <v>32.5</v>
+      </c>
+      <c r="K38" s="2">
+        <v>39.5</v>
+      </c>
+      <c r="L38" s="2"/>
+      <c r="M38" s="2"/>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A39" s="5">
+        <v>37</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C39" s="2"/>
+      <c r="D39" s="2"/>
+      <c r="E39" s="2"/>
+      <c r="F39" s="2"/>
+      <c r="G39" s="2"/>
+      <c r="H39" s="2"/>
+      <c r="I39" s="2">
+        <v>24.5</v>
+      </c>
+      <c r="J39" s="2">
+        <v>32.5</v>
+      </c>
+      <c r="K39" s="2">
+        <v>39.5</v>
+      </c>
+      <c r="L39" s="2"/>
+      <c r="M39" s="2"/>
+    </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="3">
     <mergeCell ref="C2:M2"/>
     <mergeCell ref="B6:M6"/>
-    <mergeCell ref="B19:M19"/>
     <mergeCell ref="A1:M1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
fix 10.04.2024 price 6h
</commit_message>
<xml_diff>
--- a/TeplosilaWeb/Content/properties/gtrv.xlsx
+++ b/TeplosilaWeb/Content/properties/gtrv.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Документы\ТЗ программа подбора TRV, RDT\ТЗ клапаны TRV\04.08.2023\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Документы\ТЗ программа подбора TRV, RDT\ТЗ клапаны TRV\10.04.2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="30">
   <si>
     <t>Наименование параметров,
 единицы измерения</t>
@@ -103,6 +103,18 @@
   </si>
   <si>
     <t>TSL-3000-60-2A-230-IP67</t>
+  </si>
+  <si>
+    <t>TSL-1600-25-2AR-230-IP67</t>
+  </si>
+  <si>
+    <t>TSL-1600-25-2AR-24-IP67</t>
+  </si>
+  <si>
+    <t>TSL-2200-40-2AR-230-IP67</t>
+  </si>
+  <si>
+    <t>TSL-2200-40-2AR-24-IP67</t>
   </si>
 </sst>
 </file>
@@ -211,10 +223,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -223,14 +241,8 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -512,7 +524,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N41"/>
+  <dimension ref="A1:N49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:N1"/>
@@ -526,22 +538,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11"/>
-      <c r="J1" s="11"/>
-      <c r="K1" s="11"/>
-      <c r="L1" s="11"/>
-      <c r="M1" s="11"/>
-      <c r="N1" s="11"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="13"/>
+      <c r="J1" s="13"/>
+      <c r="K1" s="13"/>
+      <c r="L1" s="13"/>
+      <c r="M1" s="13"/>
+      <c r="N1" s="13"/>
     </row>
     <row r="2" spans="1:14" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
@@ -550,26 +562,26 @@
       <c r="B2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
-      <c r="G2" s="9"/>
-      <c r="H2" s="9"/>
-      <c r="I2" s="9"/>
-      <c r="J2" s="9"/>
-      <c r="K2" s="9"/>
-      <c r="L2" s="9"/>
-      <c r="M2" s="9"/>
-      <c r="N2" s="9"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="11"/>
+      <c r="J2" s="11"/>
+      <c r="K2" s="11"/>
+      <c r="L2" s="11"/>
+      <c r="M2" s="11"/>
+      <c r="N2" s="11"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="6">
         <v>1</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="8" t="s">
         <v>2</v>
       </c>
       <c r="C3" s="4">
@@ -613,7 +625,7 @@
       <c r="A4" s="6">
         <v>2</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="8" t="s">
         <v>3</v>
       </c>
       <c r="C4" s="2">
@@ -657,7 +669,7 @@
       <c r="A5" s="6">
         <v>3</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="8" t="s">
         <v>4</v>
       </c>
       <c r="C5" s="2">
@@ -701,21 +713,21 @@
       <c r="A6" s="6">
         <v>4</v>
       </c>
-      <c r="B6" s="10" t="s">
+      <c r="B6" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="10"/>
-      <c r="D6" s="10"/>
-      <c r="E6" s="10"/>
-      <c r="F6" s="10"/>
-      <c r="G6" s="10"/>
-      <c r="H6" s="10"/>
-      <c r="I6" s="10"/>
-      <c r="J6" s="10"/>
-      <c r="K6" s="10"/>
-      <c r="L6" s="10"/>
-      <c r="M6" s="10"/>
-      <c r="N6" s="10"/>
+      <c r="C6" s="12"/>
+      <c r="D6" s="12"/>
+      <c r="E6" s="12"/>
+      <c r="F6" s="12"/>
+      <c r="G6" s="12"/>
+      <c r="H6" s="12"/>
+      <c r="I6" s="12"/>
+      <c r="J6" s="12"/>
+      <c r="K6" s="12"/>
+      <c r="L6" s="12"/>
+      <c r="M6" s="12"/>
+      <c r="N6" s="12"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="6">
@@ -817,8 +829,8 @@
       <c r="A10" s="6">
         <v>8</v>
       </c>
-      <c r="B10" s="13" t="s">
-        <v>20</v>
+      <c r="B10" s="1" t="s">
+        <v>14</v>
       </c>
       <c r="C10" s="2">
         <v>305</v>
@@ -846,173 +858,197 @@
       <c r="N10" s="2"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A11" s="12">
+      <c r="A11" s="6">
         <v>9</v>
       </c>
-      <c r="B11" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="C11" s="8">
+      <c r="B11" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" s="2">
         <v>305</v>
       </c>
-      <c r="D11" s="8">
+      <c r="D11" s="2">
         <v>305</v>
       </c>
-      <c r="E11" s="8">
+      <c r="E11" s="2">
         <v>315</v>
       </c>
-      <c r="F11" s="8">
+      <c r="F11" s="2">
         <v>325</v>
       </c>
-      <c r="G11" s="8">
+      <c r="G11" s="2">
         <v>330</v>
       </c>
-      <c r="H11" s="8">
+      <c r="H11" s="2">
         <v>340</v>
       </c>
-      <c r="I11" s="8"/>
-      <c r="J11" s="8"/>
-      <c r="K11" s="8"/>
-      <c r="L11" s="8"/>
-      <c r="M11" s="8"/>
-      <c r="N11" s="8"/>
+      <c r="I11" s="2"/>
+      <c r="J11" s="2"/>
+      <c r="K11" s="2"/>
+      <c r="L11" s="2"/>
+      <c r="M11" s="2"/>
+      <c r="N11" s="2"/>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="6">
         <v>10</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
-      <c r="H12" s="2"/>
-      <c r="I12" s="2">
-        <v>450</v>
-      </c>
-      <c r="J12" s="2">
-        <v>435</v>
-      </c>
-      <c r="K12" s="2">
-        <v>455</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="C12" s="2">
+        <v>305</v>
+      </c>
+      <c r="D12" s="2">
+        <v>305</v>
+      </c>
+      <c r="E12" s="2">
+        <v>315</v>
+      </c>
+      <c r="F12" s="2">
+        <v>325</v>
+      </c>
+      <c r="G12" s="2">
+        <v>330</v>
+      </c>
+      <c r="H12" s="2">
+        <v>340</v>
+      </c>
+      <c r="I12" s="2"/>
+      <c r="J12" s="2"/>
+      <c r="K12" s="2"/>
       <c r="L12" s="2"/>
       <c r="M12" s="2"/>
       <c r="N12" s="2"/>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A13" s="6">
+      <c r="A13" s="10">
         <v>11</v>
       </c>
-      <c r="B13" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
-      <c r="H13" s="2"/>
-      <c r="I13" s="2">
-        <v>450</v>
-      </c>
-      <c r="J13" s="2">
-        <v>435</v>
-      </c>
-      <c r="K13" s="2">
-        <v>455</v>
-      </c>
-      <c r="L13" s="2"/>
-      <c r="M13" s="2"/>
-      <c r="N13" s="2"/>
+      <c r="B13" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13" s="7">
+        <v>305</v>
+      </c>
+      <c r="D13" s="7">
+        <v>305</v>
+      </c>
+      <c r="E13" s="7">
+        <v>315</v>
+      </c>
+      <c r="F13" s="7">
+        <v>325</v>
+      </c>
+      <c r="G13" s="7">
+        <v>330</v>
+      </c>
+      <c r="H13" s="7">
+        <v>340</v>
+      </c>
+      <c r="I13" s="7"/>
+      <c r="J13" s="7"/>
+      <c r="K13" s="7"/>
+      <c r="L13" s="7"/>
+      <c r="M13" s="7"/>
+      <c r="N13" s="7"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="6">
         <v>12</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
-      <c r="H14" s="2"/>
-      <c r="I14" s="2">
-        <v>450</v>
-      </c>
-      <c r="J14" s="2">
-        <v>435</v>
-      </c>
-      <c r="K14" s="2">
-        <v>455</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="C14" s="2">
+        <v>305</v>
+      </c>
+      <c r="D14" s="2">
+        <v>305</v>
+      </c>
+      <c r="E14" s="2">
+        <v>315</v>
+      </c>
+      <c r="F14" s="2">
+        <v>325</v>
+      </c>
+      <c r="G14" s="2">
+        <v>330</v>
+      </c>
+      <c r="H14" s="2">
+        <v>340</v>
+      </c>
+      <c r="I14" s="2"/>
+      <c r="J14" s="2"/>
+      <c r="K14" s="2"/>
       <c r="L14" s="2"/>
       <c r="M14" s="2"/>
       <c r="N14" s="2"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A15" s="6">
+      <c r="A15" s="10">
         <v>13</v>
       </c>
-      <c r="B15" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
-      <c r="G15" s="2"/>
-      <c r="H15" s="2"/>
-      <c r="I15" s="2">
+      <c r="B15" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C15" s="7">
+        <v>305</v>
+      </c>
+      <c r="D15" s="7">
+        <v>305</v>
+      </c>
+      <c r="E15" s="7">
+        <v>315</v>
+      </c>
+      <c r="F15" s="7">
+        <v>325</v>
+      </c>
+      <c r="G15" s="7">
+        <v>330</v>
+      </c>
+      <c r="H15" s="7">
+        <v>340</v>
+      </c>
+      <c r="I15" s="7"/>
+      <c r="J15" s="7"/>
+      <c r="K15" s="7"/>
+      <c r="L15" s="7"/>
+      <c r="M15" s="7"/>
+      <c r="N15" s="7"/>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A16" s="6">
+        <v>14</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
+      <c r="H16" s="2"/>
+      <c r="I16" s="2">
         <v>450</v>
       </c>
-      <c r="J15" s="2">
+      <c r="J16" s="2">
         <v>435</v>
       </c>
-      <c r="K15" s="2">
+      <c r="K16" s="2">
         <v>455</v>
       </c>
-      <c r="L15" s="2"/>
-      <c r="M15" s="2"/>
-      <c r="N15" s="2"/>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A16" s="12">
-        <v>14</v>
-      </c>
-      <c r="B16" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="C16" s="8"/>
-      <c r="D16" s="8"/>
-      <c r="E16" s="8"/>
-      <c r="F16" s="8"/>
-      <c r="G16" s="8"/>
-      <c r="H16" s="8"/>
-      <c r="I16" s="8">
-        <v>450</v>
-      </c>
-      <c r="J16" s="8">
-        <v>435</v>
-      </c>
-      <c r="K16" s="8">
-        <v>455</v>
-      </c>
-      <c r="L16" s="8"/>
-      <c r="M16" s="8"/>
-      <c r="N16" s="8"/>
+      <c r="L16" s="2"/>
+      <c r="M16" s="2"/>
+      <c r="N16" s="2"/>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="6">
         <v>15</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
@@ -1020,25 +1056,25 @@
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
-      <c r="I17" s="2"/>
-      <c r="J17" s="2"/>
-      <c r="K17" s="2"/>
-      <c r="L17" s="2">
-        <v>510</v>
-      </c>
-      <c r="M17" s="2">
-        <v>515</v>
-      </c>
-      <c r="N17" s="2">
-        <v>565</v>
-      </c>
+      <c r="I17" s="2">
+        <v>450</v>
+      </c>
+      <c r="J17" s="2">
+        <v>435</v>
+      </c>
+      <c r="K17" s="2">
+        <v>455</v>
+      </c>
+      <c r="L17" s="2"/>
+      <c r="M17" s="2"/>
+      <c r="N17" s="2"/>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" s="6">
         <v>16</v>
       </c>
-      <c r="B18" s="13" t="s">
-        <v>24</v>
+      <c r="B18" s="1" t="s">
+        <v>19</v>
       </c>
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
@@ -1046,73 +1082,67 @@
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
-      <c r="I18" s="2"/>
-      <c r="J18" s="2"/>
-      <c r="K18" s="2"/>
-      <c r="L18" s="2">
-        <v>510</v>
-      </c>
-      <c r="M18" s="2">
-        <v>515</v>
-      </c>
-      <c r="N18" s="2">
-        <v>565</v>
-      </c>
+      <c r="I18" s="2">
+        <v>450</v>
+      </c>
+      <c r="J18" s="2">
+        <v>435</v>
+      </c>
+      <c r="K18" s="2">
+        <v>455</v>
+      </c>
+      <c r="L18" s="2"/>
+      <c r="M18" s="2"/>
+      <c r="N18" s="2"/>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A19" s="12">
+      <c r="A19" s="6">
         <v>17</v>
       </c>
-      <c r="B19" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="C19" s="8"/>
-      <c r="D19" s="8"/>
-      <c r="E19" s="8"/>
-      <c r="F19" s="8"/>
-      <c r="G19" s="8"/>
-      <c r="H19" s="8"/>
-      <c r="I19" s="8"/>
-      <c r="J19" s="8"/>
-      <c r="K19" s="8"/>
-      <c r="L19" s="8">
-        <v>510</v>
-      </c>
-      <c r="M19" s="8">
-        <v>515</v>
-      </c>
-      <c r="N19" s="8">
-        <v>565</v>
-      </c>
+      <c r="B19" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+      <c r="G19" s="2"/>
+      <c r="H19" s="2"/>
+      <c r="I19" s="2">
+        <v>450</v>
+      </c>
+      <c r="J19" s="2">
+        <v>435</v>
+      </c>
+      <c r="K19" s="2">
+        <v>455</v>
+      </c>
+      <c r="L19" s="2"/>
+      <c r="M19" s="2"/>
+      <c r="N19" s="2"/>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" s="6">
         <v>18</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C20" s="2">
-        <v>305</v>
-      </c>
-      <c r="D20" s="2">
-        <v>305</v>
-      </c>
-      <c r="E20" s="2">
-        <v>315</v>
-      </c>
-      <c r="F20" s="2">
-        <v>325</v>
-      </c>
-      <c r="G20" s="2">
-        <v>330</v>
-      </c>
-      <c r="H20" s="2">
-        <v>340</v>
-      </c>
-      <c r="I20" s="2"/>
-      <c r="J20" s="2"/>
-      <c r="K20" s="2"/>
+        <v>17</v>
+      </c>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
+      <c r="G20" s="2"/>
+      <c r="H20" s="2"/>
+      <c r="I20" s="2">
+        <v>450</v>
+      </c>
+      <c r="J20" s="2">
+        <v>435</v>
+      </c>
+      <c r="K20" s="2">
+        <v>455</v>
+      </c>
       <c r="L20" s="2"/>
       <c r="M20" s="2"/>
       <c r="N20" s="2"/>
@@ -1122,65 +1152,59 @@
         <v>19</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C21" s="2">
-        <v>305</v>
-      </c>
-      <c r="D21" s="2">
-        <v>305</v>
-      </c>
-      <c r="E21" s="2">
-        <v>315</v>
-      </c>
-      <c r="F21" s="2">
-        <v>325</v>
-      </c>
-      <c r="G21" s="2">
-        <v>330</v>
-      </c>
-      <c r="H21" s="2">
-        <v>340</v>
-      </c>
-      <c r="I21" s="2"/>
-      <c r="J21" s="2"/>
-      <c r="K21" s="2"/>
+        <v>23</v>
+      </c>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+      <c r="G21" s="2"/>
+      <c r="H21" s="2"/>
+      <c r="I21" s="2">
+        <v>450</v>
+      </c>
+      <c r="J21" s="2">
+        <v>435</v>
+      </c>
+      <c r="K21" s="2">
+        <v>455</v>
+      </c>
       <c r="L21" s="2"/>
       <c r="M21" s="2"/>
       <c r="N21" s="2"/>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A22" s="6">
+      <c r="A22" s="10">
         <v>20</v>
       </c>
-      <c r="B22" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
-      <c r="E22" s="2"/>
-      <c r="F22" s="2"/>
-      <c r="G22" s="2"/>
-      <c r="H22" s="2"/>
-      <c r="I22" s="2">
+      <c r="B22" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="C22" s="7"/>
+      <c r="D22" s="7"/>
+      <c r="E22" s="7"/>
+      <c r="F22" s="7"/>
+      <c r="G22" s="7"/>
+      <c r="H22" s="7"/>
+      <c r="I22" s="7">
         <v>450</v>
       </c>
-      <c r="J22" s="2">
+      <c r="J22" s="7">
         <v>435</v>
       </c>
-      <c r="K22" s="2">
+      <c r="K22" s="7">
         <v>455</v>
       </c>
-      <c r="L22" s="2"/>
-      <c r="M22" s="2"/>
-      <c r="N22" s="2"/>
+      <c r="L22" s="7"/>
+      <c r="M22" s="7"/>
+      <c r="N22" s="7"/>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" s="6">
         <v>21</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
@@ -1202,207 +1226,189 @@
       <c r="N23" s="2"/>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A24" s="6">
+      <c r="A24" s="10">
         <v>22</v>
       </c>
-      <c r="B24" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="C24" s="10"/>
-      <c r="D24" s="10"/>
-      <c r="E24" s="10"/>
-      <c r="F24" s="10"/>
-      <c r="G24" s="10"/>
-      <c r="H24" s="10"/>
-      <c r="I24" s="10"/>
-      <c r="J24" s="10"/>
-      <c r="K24" s="10"/>
-      <c r="L24" s="10"/>
-      <c r="M24" s="10"/>
-      <c r="N24" s="10"/>
+      <c r="B24" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="C24" s="7"/>
+      <c r="D24" s="7"/>
+      <c r="E24" s="7"/>
+      <c r="F24" s="7"/>
+      <c r="G24" s="7"/>
+      <c r="H24" s="7"/>
+      <c r="I24" s="7">
+        <v>450</v>
+      </c>
+      <c r="J24" s="7">
+        <v>435</v>
+      </c>
+      <c r="K24" s="7">
+        <v>455</v>
+      </c>
+      <c r="L24" s="7"/>
+      <c r="M24" s="7"/>
+      <c r="N24" s="7"/>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" s="6">
         <v>23</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C25" s="2">
-        <v>6.2</v>
-      </c>
-      <c r="D25" s="2">
-        <v>7.7</v>
-      </c>
-      <c r="E25" s="2">
-        <v>8.1999999999999993</v>
-      </c>
-      <c r="F25" s="2">
-        <v>11.2</v>
-      </c>
-      <c r="G25" s="2">
-        <v>13.2</v>
-      </c>
-      <c r="H25" s="2">
-        <v>15.2</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="C25" s="2"/>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
+      <c r="F25" s="2"/>
+      <c r="G25" s="2"/>
+      <c r="H25" s="2"/>
       <c r="I25" s="2"/>
       <c r="J25" s="2"/>
       <c r="K25" s="2"/>
-      <c r="L25" s="2"/>
-      <c r="M25" s="2"/>
-      <c r="N25" s="2"/>
+      <c r="L25" s="2">
+        <v>510</v>
+      </c>
+      <c r="M25" s="2">
+        <v>515</v>
+      </c>
+      <c r="N25" s="2">
+        <v>565</v>
+      </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" s="6">
         <v>24</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C26" s="2">
-        <v>6.2</v>
-      </c>
-      <c r="D26" s="2">
-        <v>7.7</v>
-      </c>
-      <c r="E26" s="2">
-        <v>8.1999999999999993</v>
-      </c>
-      <c r="F26" s="2">
-        <v>11.2</v>
-      </c>
-      <c r="G26" s="2">
-        <v>13.2</v>
-      </c>
-      <c r="H26" s="2">
-        <v>15.2</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="C26" s="2"/>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2"/>
+      <c r="F26" s="2"/>
+      <c r="G26" s="2"/>
+      <c r="H26" s="2"/>
       <c r="I26" s="2"/>
       <c r="J26" s="2"/>
       <c r="K26" s="2"/>
-      <c r="L26" s="2"/>
-      <c r="M26" s="2"/>
-      <c r="N26" s="2"/>
+      <c r="L26" s="2">
+        <v>510</v>
+      </c>
+      <c r="M26" s="2">
+        <v>515</v>
+      </c>
+      <c r="N26" s="2">
+        <v>565</v>
+      </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" s="6">
         <v>25</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C27" s="2">
-        <v>6.2</v>
-      </c>
-      <c r="D27" s="2">
-        <v>7.7</v>
-      </c>
-      <c r="E27" s="2">
-        <v>8.1999999999999993</v>
-      </c>
-      <c r="F27" s="2">
-        <v>11.2</v>
-      </c>
-      <c r="G27" s="2">
-        <v>13.2</v>
-      </c>
-      <c r="H27" s="2">
-        <v>15.2</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="C27" s="2"/>
+      <c r="D27" s="2"/>
+      <c r="E27" s="2"/>
+      <c r="F27" s="2"/>
+      <c r="G27" s="2"/>
+      <c r="H27" s="2"/>
       <c r="I27" s="2"/>
       <c r="J27" s="2"/>
       <c r="K27" s="2"/>
-      <c r="L27" s="2"/>
-      <c r="M27" s="2"/>
-      <c r="N27" s="2"/>
+      <c r="L27" s="2">
+        <v>510</v>
+      </c>
+      <c r="M27" s="2">
+        <v>515</v>
+      </c>
+      <c r="N27" s="2">
+        <v>565</v>
+      </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" s="6">
         <v>26</v>
       </c>
-      <c r="B28" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="C28" s="2">
+      <c r="B28" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="C28" s="12"/>
+      <c r="D28" s="12"/>
+      <c r="E28" s="12"/>
+      <c r="F28" s="12"/>
+      <c r="G28" s="12"/>
+      <c r="H28" s="12"/>
+      <c r="I28" s="12"/>
+      <c r="J28" s="12"/>
+      <c r="K28" s="12"/>
+      <c r="L28" s="12"/>
+      <c r="M28" s="12"/>
+      <c r="N28" s="12"/>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A29" s="6">
+        <v>27</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C29" s="2">
         <v>6.2</v>
       </c>
-      <c r="D28" s="2">
+      <c r="D29" s="2">
         <v>7.7</v>
       </c>
-      <c r="E28" s="2">
+      <c r="E29" s="2">
         <v>8.1999999999999993</v>
       </c>
-      <c r="F28" s="2">
+      <c r="F29" s="2">
         <v>11.2</v>
       </c>
-      <c r="G28" s="2">
+      <c r="G29" s="2">
         <v>13.2</v>
       </c>
-      <c r="H28" s="2">
+      <c r="H29" s="2">
         <v>15.2</v>
       </c>
-      <c r="I28" s="2"/>
-      <c r="J28" s="2"/>
-      <c r="K28" s="2"/>
-      <c r="L28" s="2"/>
-      <c r="M28" s="2"/>
-      <c r="N28" s="2"/>
-    </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A29" s="12">
-        <v>27</v>
-      </c>
-      <c r="B29" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="C29" s="8">
-        <v>6.2</v>
-      </c>
-      <c r="D29" s="8">
-        <v>7.7</v>
-      </c>
-      <c r="E29" s="8">
-        <v>8.1999999999999993</v>
-      </c>
-      <c r="F29" s="8">
-        <v>11.2</v>
-      </c>
-      <c r="G29" s="8">
-        <v>13.2</v>
-      </c>
-      <c r="H29" s="8">
-        <v>15.2</v>
-      </c>
-      <c r="I29" s="8"/>
-      <c r="J29" s="8"/>
-      <c r="K29" s="8"/>
-      <c r="L29" s="8"/>
-      <c r="M29" s="8"/>
-      <c r="N29" s="8"/>
+      <c r="I29" s="2"/>
+      <c r="J29" s="2"/>
+      <c r="K29" s="2"/>
+      <c r="L29" s="2"/>
+      <c r="M29" s="2"/>
+      <c r="N29" s="2"/>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" s="6">
         <v>28</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C30" s="2"/>
-      <c r="D30" s="2"/>
-      <c r="E30" s="2"/>
-      <c r="F30" s="2"/>
-      <c r="G30" s="2"/>
-      <c r="H30" s="2"/>
-      <c r="I30" s="2">
-        <v>23.9</v>
-      </c>
-      <c r="J30" s="2">
-        <v>28.6</v>
-      </c>
-      <c r="K30" s="2">
-        <v>33.9</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="C30" s="2">
+        <v>6.2</v>
+      </c>
+      <c r="D30" s="2">
+        <v>7.7</v>
+      </c>
+      <c r="E30" s="2">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="F30" s="2">
+        <v>11.2</v>
+      </c>
+      <c r="G30" s="2">
+        <v>13.2</v>
+      </c>
+      <c r="H30" s="2">
+        <v>15.2</v>
+      </c>
+      <c r="I30" s="2"/>
+      <c r="J30" s="2"/>
+      <c r="K30" s="2"/>
       <c r="L30" s="2"/>
       <c r="M30" s="2"/>
       <c r="N30" s="2"/>
@@ -1412,23 +1418,29 @@
         <v>29</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C31" s="2"/>
-      <c r="D31" s="2"/>
-      <c r="E31" s="2"/>
-      <c r="F31" s="2"/>
-      <c r="G31" s="2"/>
-      <c r="H31" s="2"/>
-      <c r="I31" s="2">
-        <v>23.9</v>
-      </c>
-      <c r="J31" s="2">
-        <v>28.6</v>
-      </c>
-      <c r="K31" s="2">
-        <v>33.9</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="C31" s="2">
+        <v>6.2</v>
+      </c>
+      <c r="D31" s="2">
+        <v>7.7</v>
+      </c>
+      <c r="E31" s="2">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="F31" s="2">
+        <v>11.2</v>
+      </c>
+      <c r="G31" s="2">
+        <v>13.2</v>
+      </c>
+      <c r="H31" s="2">
+        <v>15.2</v>
+      </c>
+      <c r="I31" s="2"/>
+      <c r="J31" s="2"/>
+      <c r="K31" s="2"/>
       <c r="L31" s="2"/>
       <c r="M31" s="2"/>
       <c r="N31" s="2"/>
@@ -1438,23 +1450,29 @@
         <v>30</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C32" s="2"/>
-      <c r="D32" s="2"/>
-      <c r="E32" s="2"/>
-      <c r="F32" s="2"/>
-      <c r="G32" s="2"/>
-      <c r="H32" s="2"/>
-      <c r="I32" s="2">
-        <v>23.9</v>
-      </c>
-      <c r="J32" s="2">
-        <v>28.6</v>
-      </c>
-      <c r="K32" s="2">
-        <v>33.9</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="C32" s="2">
+        <v>6.2</v>
+      </c>
+      <c r="D32" s="2">
+        <v>7.7</v>
+      </c>
+      <c r="E32" s="2">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="F32" s="2">
+        <v>11.2</v>
+      </c>
+      <c r="G32" s="2">
+        <v>13.2</v>
+      </c>
+      <c r="H32" s="2">
+        <v>15.2</v>
+      </c>
+      <c r="I32" s="2"/>
+      <c r="J32" s="2"/>
+      <c r="K32" s="2"/>
       <c r="L32" s="2"/>
       <c r="M32" s="2"/>
       <c r="N32" s="2"/>
@@ -1463,160 +1481,184 @@
       <c r="A33" s="6">
         <v>31</v>
       </c>
-      <c r="B33" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="C33" s="2"/>
-      <c r="D33" s="2"/>
-      <c r="E33" s="2"/>
-      <c r="F33" s="2"/>
-      <c r="G33" s="2"/>
-      <c r="H33" s="2"/>
-      <c r="I33" s="2">
-        <v>23.9</v>
-      </c>
-      <c r="J33" s="2">
-        <v>28.6</v>
-      </c>
-      <c r="K33" s="2">
-        <v>33.9</v>
-      </c>
+      <c r="B33" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C33" s="2">
+        <v>6.2</v>
+      </c>
+      <c r="D33" s="2">
+        <v>7.7</v>
+      </c>
+      <c r="E33" s="2">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="F33" s="2">
+        <v>11.2</v>
+      </c>
+      <c r="G33" s="2">
+        <v>13.2</v>
+      </c>
+      <c r="H33" s="2">
+        <v>15.2</v>
+      </c>
+      <c r="I33" s="2"/>
+      <c r="J33" s="2"/>
+      <c r="K33" s="2"/>
       <c r="L33" s="2"/>
       <c r="M33" s="2"/>
       <c r="N33" s="2"/>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A34" s="12">
+      <c r="A34" s="6">
         <v>32</v>
       </c>
-      <c r="B34" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="C34" s="8"/>
-      <c r="D34" s="8"/>
-      <c r="E34" s="8"/>
-      <c r="F34" s="8"/>
-      <c r="G34" s="8"/>
-      <c r="H34" s="8"/>
-      <c r="I34" s="8">
-        <v>23.9</v>
-      </c>
-      <c r="J34" s="8">
-        <v>28.6</v>
-      </c>
-      <c r="K34" s="8">
-        <v>33.9</v>
-      </c>
-      <c r="L34" s="8"/>
-      <c r="M34" s="8"/>
-      <c r="N34" s="8"/>
+      <c r="B34" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C34" s="2">
+        <v>6.2</v>
+      </c>
+      <c r="D34" s="2">
+        <v>7.7</v>
+      </c>
+      <c r="E34" s="2">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="F34" s="2">
+        <v>11.2</v>
+      </c>
+      <c r="G34" s="2">
+        <v>13.2</v>
+      </c>
+      <c r="H34" s="2">
+        <v>15.2</v>
+      </c>
+      <c r="I34" s="2"/>
+      <c r="J34" s="2"/>
+      <c r="K34" s="2"/>
+      <c r="L34" s="2"/>
+      <c r="M34" s="2"/>
+      <c r="N34" s="2"/>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A35" s="6">
+      <c r="A35" s="10">
         <v>33</v>
       </c>
-      <c r="B35" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C35" s="2"/>
-      <c r="D35" s="2"/>
-      <c r="E35" s="2"/>
-      <c r="F35" s="2"/>
-      <c r="G35" s="2"/>
-      <c r="H35" s="2"/>
-      <c r="I35" s="2"/>
-      <c r="J35" s="2"/>
-      <c r="K35" s="2"/>
-      <c r="L35" s="2">
-        <v>46</v>
-      </c>
-      <c r="M35" s="2">
-        <v>58.9</v>
-      </c>
-      <c r="N35" s="2">
-        <v>59.3</v>
-      </c>
+      <c r="B35" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C35" s="7">
+        <v>6.2</v>
+      </c>
+      <c r="D35" s="7">
+        <v>7.7</v>
+      </c>
+      <c r="E35" s="7">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="F35" s="7">
+        <v>11.2</v>
+      </c>
+      <c r="G35" s="7">
+        <v>13.2</v>
+      </c>
+      <c r="H35" s="7">
+        <v>15.2</v>
+      </c>
+      <c r="I35" s="7"/>
+      <c r="J35" s="7"/>
+      <c r="K35" s="7"/>
+      <c r="L35" s="7"/>
+      <c r="M35" s="7"/>
+      <c r="N35" s="7"/>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A36" s="6">
         <v>34</v>
       </c>
-      <c r="B36" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="C36" s="2"/>
-      <c r="D36" s="2"/>
-      <c r="E36" s="2"/>
-      <c r="F36" s="2"/>
-      <c r="G36" s="2"/>
-      <c r="H36" s="2"/>
+      <c r="B36" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C36" s="2">
+        <v>6.2</v>
+      </c>
+      <c r="D36" s="2">
+        <v>7.7</v>
+      </c>
+      <c r="E36" s="2">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="F36" s="2">
+        <v>11.2</v>
+      </c>
+      <c r="G36" s="2">
+        <v>13.2</v>
+      </c>
+      <c r="H36" s="2">
+        <v>15.2</v>
+      </c>
       <c r="I36" s="2"/>
       <c r="J36" s="2"/>
       <c r="K36" s="2"/>
-      <c r="L36" s="2">
-        <v>46</v>
-      </c>
-      <c r="M36" s="2">
-        <v>58.9</v>
-      </c>
-      <c r="N36" s="2">
-        <v>59.3</v>
-      </c>
+      <c r="L36" s="2"/>
+      <c r="M36" s="2"/>
+      <c r="N36" s="2"/>
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A37" s="12">
+      <c r="A37" s="10">
         <v>35</v>
       </c>
-      <c r="B37" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="C37" s="8"/>
-      <c r="D37" s="8"/>
-      <c r="E37" s="8"/>
-      <c r="F37" s="8"/>
-      <c r="G37" s="8"/>
-      <c r="H37" s="8"/>
-      <c r="I37" s="8"/>
-      <c r="J37" s="8"/>
-      <c r="K37" s="8"/>
-      <c r="L37" s="8">
-        <v>46</v>
-      </c>
-      <c r="M37" s="8">
-        <v>58.9</v>
-      </c>
-      <c r="N37" s="8">
-        <v>59.3</v>
-      </c>
+      <c r="B37" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C37" s="7">
+        <v>6.2</v>
+      </c>
+      <c r="D37" s="7">
+        <v>7.7</v>
+      </c>
+      <c r="E37" s="7">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="F37" s="7">
+        <v>11.2</v>
+      </c>
+      <c r="G37" s="7">
+        <v>13.2</v>
+      </c>
+      <c r="H37" s="7">
+        <v>15.2</v>
+      </c>
+      <c r="I37" s="7"/>
+      <c r="J37" s="7"/>
+      <c r="K37" s="7"/>
+      <c r="L37" s="7"/>
+      <c r="M37" s="7"/>
+      <c r="N37" s="7"/>
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A38" s="6">
         <v>36</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C38" s="2">
-        <v>6.2</v>
-      </c>
-      <c r="D38" s="2">
-        <v>7.7</v>
-      </c>
-      <c r="E38" s="2">
-        <v>8.1999999999999993</v>
-      </c>
-      <c r="F38" s="2">
-        <v>11.2</v>
-      </c>
-      <c r="G38" s="2">
-        <v>13.2</v>
-      </c>
-      <c r="H38" s="2">
-        <v>15.2</v>
-      </c>
-      <c r="I38" s="2"/>
-      <c r="J38" s="2"/>
-      <c r="K38" s="2"/>
+        <v>7</v>
+      </c>
+      <c r="C38" s="2"/>
+      <c r="D38" s="2"/>
+      <c r="E38" s="2"/>
+      <c r="F38" s="2"/>
+      <c r="G38" s="2"/>
+      <c r="H38" s="2"/>
+      <c r="I38" s="2">
+        <v>23.9</v>
+      </c>
+      <c r="J38" s="2">
+        <v>28.6</v>
+      </c>
+      <c r="K38" s="2">
+        <v>33.9</v>
+      </c>
       <c r="L38" s="2"/>
       <c r="M38" s="2"/>
       <c r="N38" s="2"/>
@@ -1626,29 +1668,23 @@
         <v>37</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C39" s="2">
-        <v>6.2</v>
-      </c>
-      <c r="D39" s="2">
-        <v>7.7</v>
-      </c>
-      <c r="E39" s="2">
-        <v>8.1999999999999993</v>
-      </c>
-      <c r="F39" s="2">
-        <v>11.2</v>
-      </c>
-      <c r="G39" s="2">
-        <v>13.2</v>
-      </c>
-      <c r="H39" s="2">
-        <v>15.2</v>
-      </c>
-      <c r="I39" s="2"/>
-      <c r="J39" s="2"/>
-      <c r="K39" s="2"/>
+        <v>8</v>
+      </c>
+      <c r="C39" s="2"/>
+      <c r="D39" s="2"/>
+      <c r="E39" s="2"/>
+      <c r="F39" s="2"/>
+      <c r="G39" s="2"/>
+      <c r="H39" s="2"/>
+      <c r="I39" s="2">
+        <v>23.9</v>
+      </c>
+      <c r="J39" s="2">
+        <v>28.6</v>
+      </c>
+      <c r="K39" s="2">
+        <v>33.9</v>
+      </c>
       <c r="L39" s="2"/>
       <c r="M39" s="2"/>
       <c r="N39" s="2"/>
@@ -1658,7 +1694,7 @@
         <v>38</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C40" s="2"/>
       <c r="D40" s="2"/>
@@ -1684,7 +1720,7 @@
         <v>39</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C41" s="2"/>
       <c r="D41" s="2"/>
@@ -1705,11 +1741,219 @@
       <c r="M41" s="2"/>
       <c r="N41" s="2"/>
     </row>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A42" s="6">
+        <v>40</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C42" s="2"/>
+      <c r="D42" s="2"/>
+      <c r="E42" s="2"/>
+      <c r="F42" s="2"/>
+      <c r="G42" s="2"/>
+      <c r="H42" s="2"/>
+      <c r="I42" s="2">
+        <v>23.9</v>
+      </c>
+      <c r="J42" s="2">
+        <v>28.6</v>
+      </c>
+      <c r="K42" s="2">
+        <v>33.9</v>
+      </c>
+      <c r="L42" s="2"/>
+      <c r="M42" s="2"/>
+      <c r="N42" s="2"/>
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A43" s="6">
+        <v>41</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C43" s="2"/>
+      <c r="D43" s="2"/>
+      <c r="E43" s="2"/>
+      <c r="F43" s="2"/>
+      <c r="G43" s="2"/>
+      <c r="H43" s="2"/>
+      <c r="I43" s="2">
+        <v>23.9</v>
+      </c>
+      <c r="J43" s="2">
+        <v>28.6</v>
+      </c>
+      <c r="K43" s="2">
+        <v>33.9</v>
+      </c>
+      <c r="L43" s="2"/>
+      <c r="M43" s="2"/>
+      <c r="N43" s="2"/>
+    </row>
+    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A44" s="10">
+        <v>42</v>
+      </c>
+      <c r="B44" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="C44" s="7"/>
+      <c r="D44" s="7"/>
+      <c r="E44" s="7"/>
+      <c r="F44" s="7"/>
+      <c r="G44" s="7"/>
+      <c r="H44" s="7"/>
+      <c r="I44" s="7">
+        <v>23.9</v>
+      </c>
+      <c r="J44" s="7">
+        <v>28.6</v>
+      </c>
+      <c r="K44" s="7">
+        <v>33.9</v>
+      </c>
+      <c r="L44" s="7"/>
+      <c r="M44" s="7"/>
+      <c r="N44" s="7"/>
+    </row>
+    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A45" s="6">
+        <v>43</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C45" s="2"/>
+      <c r="D45" s="2"/>
+      <c r="E45" s="2"/>
+      <c r="F45" s="2"/>
+      <c r="G45" s="2"/>
+      <c r="H45" s="2"/>
+      <c r="I45" s="2">
+        <v>23.9</v>
+      </c>
+      <c r="J45" s="2">
+        <v>28.6</v>
+      </c>
+      <c r="K45" s="2">
+        <v>33.9</v>
+      </c>
+      <c r="L45" s="2"/>
+      <c r="M45" s="2"/>
+      <c r="N45" s="2"/>
+    </row>
+    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A46" s="10">
+        <v>44</v>
+      </c>
+      <c r="B46" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="C46" s="7"/>
+      <c r="D46" s="7"/>
+      <c r="E46" s="7"/>
+      <c r="F46" s="7"/>
+      <c r="G46" s="7"/>
+      <c r="H46" s="7"/>
+      <c r="I46" s="7">
+        <v>23.9</v>
+      </c>
+      <c r="J46" s="7">
+        <v>28.6</v>
+      </c>
+      <c r="K46" s="7">
+        <v>33.9</v>
+      </c>
+      <c r="L46" s="7"/>
+      <c r="M46" s="7"/>
+      <c r="N46" s="7"/>
+    </row>
+    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A47" s="6">
+        <v>45</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C47" s="2"/>
+      <c r="D47" s="2"/>
+      <c r="E47" s="2"/>
+      <c r="F47" s="2"/>
+      <c r="G47" s="2"/>
+      <c r="H47" s="2"/>
+      <c r="I47" s="2"/>
+      <c r="J47" s="2"/>
+      <c r="K47" s="2"/>
+      <c r="L47" s="2">
+        <v>46</v>
+      </c>
+      <c r="M47" s="2">
+        <v>58.9</v>
+      </c>
+      <c r="N47" s="2">
+        <v>59.3</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A48" s="6">
+        <v>46</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C48" s="2"/>
+      <c r="D48" s="2"/>
+      <c r="E48" s="2"/>
+      <c r="F48" s="2"/>
+      <c r="G48" s="2"/>
+      <c r="H48" s="2"/>
+      <c r="I48" s="2"/>
+      <c r="J48" s="2"/>
+      <c r="K48" s="2"/>
+      <c r="L48" s="2">
+        <v>46</v>
+      </c>
+      <c r="M48" s="2">
+        <v>58.9</v>
+      </c>
+      <c r="N48" s="2">
+        <v>59.3</v>
+      </c>
+    </row>
+    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A49" s="6">
+        <v>47</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C49" s="2"/>
+      <c r="D49" s="2"/>
+      <c r="E49" s="2"/>
+      <c r="F49" s="2"/>
+      <c r="G49" s="2"/>
+      <c r="H49" s="2"/>
+      <c r="I49" s="2"/>
+      <c r="J49" s="2"/>
+      <c r="K49" s="2"/>
+      <c r="L49" s="2">
+        <v>46</v>
+      </c>
+      <c r="M49" s="2">
+        <v>58.9</v>
+      </c>
+      <c r="N49" s="2">
+        <v>59.3</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="C2:N2"/>
     <mergeCell ref="B6:N6"/>
-    <mergeCell ref="B24:N24"/>
+    <mergeCell ref="B28:N28"/>
     <mergeCell ref="A1:N1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>